<commit_message>
Updated relative_weights to v3
After speaking with someone who took the course in the past I have
rearranged the weights appropriately.
</commit_message>
<xml_diff>
--- a/docs/relative_weights.xlsx
+++ b/docs/relative_weights.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>local variables</t>
   </si>
@@ -130,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,8 +181,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -190,8 +203,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,14 +245,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,22 +603,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1">
+    <row r="1" spans="1:9" ht="16" thickBot="1">
       <c r="A1" s="9">
         <v>1</v>
       </c>
@@ -588,13 +635,16 @@
       <c r="E1" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="F1" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>9</v>
@@ -605,8 +655,11 @@
       <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" thickBot="1">
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -620,10 +673,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -639,8 +695,11 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1">
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -653,25 +712,28 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>3</v>
       </c>
       <c r="B6" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="8">
         <f>0</f>
@@ -682,64 +744,67 @@
         <v>5</v>
       </c>
       <c r="E6" s="8">
-        <v>28</v>
-      </c>
-      <c r="F6" s="5">
-        <f>(E6+D6+C6+B6+A6)+7</f>
-        <v>45</v>
-      </c>
-      <c r="G6" s="7">
-        <f>ROUNDUP(F6/4,0)</f>
-        <v>12</v>
-      </c>
-      <c r="H6" s="6">
-        <f>ROUNDUP(G6/3,0)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5">
+        <f>(E6+D6+C6+B6+A6+F6)+9</f>
+        <v>60</v>
+      </c>
+      <c r="H6" s="7">
+        <f>ROUNDUP(G6/4,0)</f>
+        <v>15</v>
+      </c>
+      <c r="I6" s="6">
+        <f>ROUNDUP(H6/3,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>